<commit_message>
basic download feature done
</commit_message>
<xml_diff>
--- a/Student-Distributor/src/Excel/schedule_final .xlsx
+++ b/Student-Distributor/src/Excel/schedule_final .xlsx
@@ -712,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="10">
-        <v>2.416666666666667</v>
+        <v>3.4166666666666665</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>11</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="10">
-        <v>2.416666666666667</v>
+        <v>3.4166666666666665</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>11</v>
@@ -752,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="14">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>11</v>
@@ -771,7 +771,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="14">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>11</v>
@@ -792,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="17">
-        <v>2.583333333333333</v>
+        <v>3.5833333333333335</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>11</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="10">
-        <v>2.416666666666667</v>
+        <v>3.4166666666666665</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>11</v>
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="10">
-        <v>2.416666666666667</v>
+        <v>3.4166666666666665</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>11</v>
@@ -864,7 +864,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="14">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>11</v>
@@ -885,7 +885,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="14">
-        <v>2.583333333333333</v>
+        <v>3.5833333333333335</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>11</v>
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="17">
-        <v>2.583333333333333</v>
+        <v>3.5833333333333335</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>11</v>

</xml_diff>